<commit_message>
Updated CQL and example
</commit_message>
<xml_diff>
--- a/input/l2/DTR.xlsx
+++ b/input/l2/DTR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryn\Documents\Src\Alphora\dtr-content-r4\input\l2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA653BC-2115-4B9E-A983-ABD3C2BAECCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23482CA8-73CC-4D56-B043-628E519164F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7905" yWindow="2115" windowWidth="19200" windowHeight="10395" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5932" yWindow="1590" windowWidth="19201" windowHeight="10395" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -4248,10 +4248,10 @@
   <dimension ref="A1:BR155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="V1" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>

</xml_diff>